<commit_message>
updated reeds deployment curve
and finished modifying scenarios. now to figure out bifi factors and run simulation
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/SF_reeds_alternates.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/SF_reeds_alternates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFF9C1B-CE75-47E0-B3AE-84D416FE2A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EA6531-8D91-43C8-88F1-4CEC537476EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1130" yWindow="0" windowWidth="10510" windowHeight="9550" xr2:uid="{EE4946D5-19DF-402E-8CBF-C0743D484095}"/>
+    <workbookView xWindow="42585" yWindow="-3420" windowWidth="9600" windowHeight="10245" xr2:uid="{EE4946D5-19DF-402E-8CBF-C0743D484095}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,14 +52,17 @@
     <t>expo decay hitting at least 2050 target</t>
   </si>
   <si>
-    <t>already installed</t>
+    <t>Historically annual</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,8 +78,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,8 +116,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -98,17 +131,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="%" xfId="3" xr:uid="{B5534A7B-088A-486F-9D1A-868DE4976B2B}"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma 11 4 4" xfId="2" xr:uid="{BB3266FC-0940-4F13-98C2-515AC3F194C4}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 237" xfId="6" xr:uid="{7FF99C63-95BF-422E-AF9F-42659FD07164}"/>
+    <cellStyle name="Normal 238" xfId="5" xr:uid="{C5BC32B6-F3FF-43CA-91D6-443C1F8DF2DF}"/>
+    <cellStyle name="Normal 239" xfId="4" xr:uid="{51F120FA-6A9D-4733-B47B-5CBD9E2E9EAD}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -121,6 +185,1495 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$6:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>24236.415969999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24236.415969999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74146.088489999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74146.088489999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57401.30156</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57401.30156</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>81197.986510000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>81197.986510000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>66012.061780000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>66012.061780000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>59935.855219999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>59935.855219999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>67039.351509999993</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>67039.351509999993</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>78553.287849999993</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>78553.287849999993</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>87426.894740000003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>87426.894740000003</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26258.301319999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26258.301319999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>23596.72896</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23596.72896</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>29613.993350000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>29613.993350000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>35203.627130000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>35203.627130000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>51033.75604</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>51033.75604</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5300-4742-95CF-ED7343ED0750}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$6:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$6:$F$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>42000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5300-4742-95CF-ED7343ED0750}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$6:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$6:$H$33</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>51427.574280000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51703.88175</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51991.995949999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52292.896699999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>52607.68778</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>52937.618459999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>53284.109839999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>53648.78746</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>54033.521890000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>54440.479890000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>54872.189429999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55331.623570000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>55822.309849999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>56348.475149999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>56915.240810000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>57528.890140000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>58197.243069999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>58930.193500000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>59740.50157</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>60645.000390000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>61666.50561</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>62836.980759999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>64203.092270000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>65836.690239999996</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>67856.556570000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>70479.893379999994</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>74170.972640000007</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>80250.092520000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5300-4742-95CF-ED7343ED0750}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="613424448"/>
+        <c:axId val="613431008"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="613424448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="613431008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="613431008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="613424448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>314324</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>30162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDDF0F78-CC7D-E062-03E9-4206F7526A73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -423,12 +1976,13 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
@@ -444,6 +1998,9 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
       <c r="H1" t="s">
         <v>4</v>
       </c>
@@ -452,6 +2009,9 @@
       <c r="A2">
         <v>2019</v>
       </c>
+      <c r="G2" s="7">
+        <v>13536.696959021681</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -468,6 +2028,9 @@
         <f>(E8-E3)/(B8-B3)</f>
         <v>42000</v>
       </c>
+      <c r="G3" s="7">
+        <v>19914.550100562494</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -480,24 +2043,33 @@
       <c r="F4">
         <v>42000</v>
       </c>
+      <c r="G4" s="7">
+        <v>24094.804465238103</v>
+      </c>
       <c r="H4">
         <v>100000</v>
       </c>
-      <c r="I4" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>2022</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F5">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3">
         <v>42000</v>
       </c>
+      <c r="G5" s="8">
+        <v>21893.147053291963</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
@@ -507,10 +2079,10 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <v>24236.415969999998</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="4">
         <f>C$34/28</f>
         <v>54403.97503071426</v>
       </c>
@@ -518,8 +2090,8 @@
       <c r="F6" s="1">
         <v>42000</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1">
+      <c r="G6" s="6"/>
+      <c r="H6" s="4">
         <v>51427.574280000001</v>
       </c>
       <c r="I6" s="1"/>
@@ -533,10 +2105,10 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="5">
         <v>24236.415969999998</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="5">
         <f t="shared" ref="D7:D33" si="1">C$34/28</f>
         <v>54403.97503071426</v>
       </c>
@@ -547,7 +2119,7 @@
         <f>SUM(F3:F7)+E3</f>
         <v>225000</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="5">
         <v>51703.88175</v>
       </c>
     </row>
@@ -559,10 +2131,10 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>74146.088489999995</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
@@ -573,7 +2145,7 @@
         <f>(E13-E8)/(B13-B8)</f>
         <v>65000</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="5">
         <v>51991.995949999997</v>
       </c>
     </row>
@@ -585,17 +2157,17 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="5">
         <v>74146.088489999995</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F9">
         <v>65000</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="5">
         <v>52292.896699999998</v>
       </c>
     </row>
@@ -607,17 +2179,17 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>57401.30156</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F10">
         <v>65000</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="5">
         <v>52607.68778</v>
       </c>
     </row>
@@ -629,17 +2201,17 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <v>57401.30156</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F11">
         <v>65000</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="5">
         <v>52937.618459999998</v>
       </c>
     </row>
@@ -651,10 +2223,10 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>81197.986510000002</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
@@ -665,7 +2237,7 @@
         <f>SUM(F3:F12)+E3</f>
         <v>550000</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="5">
         <v>53284.109839999997</v>
       </c>
     </row>
@@ -677,10 +2249,10 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <v>81197.986510000002</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
@@ -691,7 +2263,7 @@
         <f>(E18-E13)/(B18-B13)</f>
         <v>90000</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="5">
         <v>53648.78746</v>
       </c>
     </row>
@@ -703,17 +2275,17 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="5">
         <v>66012.061780000004</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F14">
         <v>90000</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="5">
         <v>54033.521890000004</v>
       </c>
     </row>
@@ -725,17 +2297,17 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="5">
         <v>66012.061780000004</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F15">
         <v>90000</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="5">
         <v>54440.479890000002</v>
       </c>
     </row>
@@ -747,17 +2319,17 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="5">
         <v>59935.855219999998</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F16">
         <v>90000</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="5">
         <v>54872.189429999999</v>
       </c>
     </row>
@@ -769,10 +2341,10 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="5">
         <v>59935.855219999998</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
@@ -783,7 +2355,7 @@
         <f>SUM(F3:F17,E3)</f>
         <v>1000000</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="5">
         <v>55331.623570000003</v>
       </c>
     </row>
@@ -795,10 +2367,10 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="5">
         <v>67039.351509999993</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
@@ -809,7 +2381,7 @@
         <f>(E33-E18)/(B33-B18)</f>
         <v>40000</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="5">
         <v>55822.309849999998</v>
       </c>
     </row>
@@ -821,17 +2393,17 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="5">
         <v>67039.351509999993</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F19">
         <v>40000</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="5">
         <v>56348.475149999998</v>
       </c>
     </row>
@@ -843,17 +2415,17 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="5">
         <v>78553.287849999993</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F20">
         <v>40000</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="5">
         <v>56915.240810000003</v>
       </c>
     </row>
@@ -865,17 +2437,17 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="5">
         <v>78553.287849999993</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F21">
         <v>40000</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="5">
         <v>57528.890140000003</v>
       </c>
     </row>
@@ -887,17 +2459,17 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="5">
         <v>87426.894740000003</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F22">
         <v>40000</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="5">
         <v>58197.243069999997</v>
       </c>
     </row>
@@ -909,17 +2481,17 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="5">
         <v>87426.894740000003</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F23">
         <v>40000</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="5">
         <v>58930.193500000001</v>
       </c>
     </row>
@@ -931,17 +2503,17 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="5">
         <v>26258.301319999999</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F24">
         <v>40000</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="5">
         <v>59740.50157</v>
       </c>
     </row>
@@ -953,17 +2525,17 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="5">
         <v>26258.301319999999</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F25">
         <v>40000</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="5">
         <v>60645.000390000001</v>
       </c>
     </row>
@@ -975,17 +2547,17 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="5">
         <v>23596.72896</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F26">
         <v>40000</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="5">
         <v>61666.50561</v>
       </c>
     </row>
@@ -997,17 +2569,17 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="5">
         <v>23596.72896</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F27">
         <v>40000</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="5">
         <v>62836.980759999999</v>
       </c>
     </row>
@@ -1019,17 +2591,17 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="5">
         <v>29613.993350000001</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F28">
         <v>40000</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="5">
         <v>64203.092270000001</v>
       </c>
     </row>
@@ -1041,17 +2613,17 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="5">
         <v>29613.993350000001</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F29">
         <v>40000</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="5">
         <v>65836.690239999996</v>
       </c>
     </row>
@@ -1063,17 +2635,17 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="5">
         <v>35203.627130000001</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F30">
         <v>40000</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="5">
         <v>67856.556570000001</v>
       </c>
     </row>
@@ -1085,17 +2657,17 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="5">
         <v>35203.627130000001</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F31">
         <v>40000</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="5">
         <v>70479.893379999994</v>
       </c>
     </row>
@@ -1107,21 +2679,17 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="5">
         <v>51033.75604</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="F32">
         <v>40000</v>
       </c>
-      <c r="G32">
-        <f>SUM(F3:F32,E3)</f>
-        <v>1600000</v>
-      </c>
-      <c r="H32">
+      <c r="H32" s="5">
         <v>74170.972640000007</v>
       </c>
     </row>
@@ -1133,17 +2701,24 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="5">
         <v>51033.75604</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="5">
         <f t="shared" si="1"/>
         <v>54403.97503071426</v>
       </c>
       <c r="E33">
         <v>1600000</v>
       </c>
-      <c r="H33">
+      <c r="F33">
+        <v>40000</v>
+      </c>
+      <c r="G33">
+        <f>SUM(F3:F33,E3)</f>
+        <v>1640000</v>
+      </c>
+      <c r="H33" s="5">
         <v>80250.092520000006</v>
       </c>
     </row>
@@ -1158,13 +2733,18 @@
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2">
-        <f>SUM(F3:F32)</f>
-        <v>1585000</v>
+        <f>SUM(F6:F33)</f>
+        <v>1499000</v>
       </c>
       <c r="G34" s="2"/>
+      <c r="H34" s="2">
+        <f>SUM(H6:H33)</f>
+        <v>1650001.00547</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>